<commit_message>
podmiana pliku tabela xlsx
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.tokarska\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kryst\PycharmProjects\TekstyAlternatywne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE201FF-4D4A-4269-828A-E8E6CDD301B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221BB9AE-B363-40E3-8914-6757F292B352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2265" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Krysia</t>
   </si>
@@ -55,15 +55,6 @@
   </si>
   <si>
     <t>Zdecydowanie nie</t>
-  </si>
-  <si>
-    <t>Tak</t>
-  </si>
-  <si>
-    <t>Nie</t>
-  </si>
-  <si>
-    <t>Nie wiem</t>
   </si>
 </sst>
 </file>
@@ -107,12 +98,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -394,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -416,7 +405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -433,7 +422,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -450,7 +439,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -467,7 +456,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -484,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -501,7 +490,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -517,144 +506,6 @@
       <c r="E7" s="2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>3</v>
-      </c>
-      <c r="E9" s="4">
-        <v>4</v>
-      </c>
-      <c r="F9" s="4">
-        <v>5</v>
-      </c>
-      <c r="G9" s="4">
-        <v>6</v>
-      </c>
-      <c r="H9" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.99</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>